<commit_message>
IS labs 1, 2
</commit_message>
<xml_diff>
--- a/Shandra/Plan.xlsx
+++ b/Shandra/Plan.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Автор</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0" shapeId="0">
@@ -29,7 +29,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -179,7 +179,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -230,7 +230,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -256,7 +256,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -632,15 +632,15 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="20% - Accent6" xfId="8" builtinId="50"/>
-    <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
-    <cellStyle name="Accent4" xfId="7" builtinId="41"/>
-    <cellStyle name="Bad" xfId="6" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
-    <cellStyle name="Good" xfId="4" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
+    <cellStyle name="20% – Акцентування6" xfId="8" builtinId="50"/>
+    <cellStyle name="60% – Акцентування5" xfId="5" builtinId="48"/>
+    <cellStyle name="Акцентування4" xfId="7" builtinId="41"/>
+    <cellStyle name="Гарний" xfId="4" builtinId="26"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Контрольна клітинка" xfId="2" builtinId="23"/>
+    <cellStyle name="Обчислення" xfId="1" builtinId="22"/>
+    <cellStyle name="Поганий" xfId="6" builtinId="27"/>
+    <cellStyle name="Примітка" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -656,7 +656,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -945,7 +945,7 @@
   <dimension ref="B1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1033,7 @@
       <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>5</v>
       </c>
       <c r="I4" s="11" t="s">
@@ -1070,7 +1070,7 @@
       <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>5</v>
       </c>
       <c r="I5" s="2"/>

</xml_diff>